<commit_message>
Emp_title traitement et dictionnaire
</commit_message>
<xml_diff>
--- a/Dictionary.xlsx
+++ b/Dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morga\OneDrive\Documents\MASTER\Programmation_S2\PROJET\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8333b86f315e616d/Documents/MASTER/Programmation_S2/PROJET/loan_investments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F23C249-500D-409D-B8E8-C81E2494DB2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{3F23C249-500D-409D-B8E8-C81E2494DB2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{795087F8-5917-4BE6-A8DE-18F4BCA5654A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4339708A-1039-4E3E-98B0-F6367F6FEB2C}"/>
+    <workbookView xWindow="-220" yWindow="1180" windowWidth="5390" windowHeight="7360" xr2:uid="{4339708A-1039-4E3E-98B0-F6367F6FEB2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="304">
   <si>
     <t>id</t>
   </si>
@@ -923,6 +923,21 @@
   </si>
   <si>
     <t>//</t>
+  </si>
+  <si>
+    <t>36 ou 60 paiements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le score se fait au moment du prêt donc l'info sera bonne </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bonne variable </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Info données </t>
+  </si>
+  <si>
+    <t>Il peut y avoir des données interessantes par états</t>
   </si>
 </sst>
 </file>
@@ -1066,7 +1081,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1252,6 +1267,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -1428,22 +1479,65 @@
     <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="32">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="17" builtinId="30" customBuiltin="1"/>
@@ -1801,48 +1895,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3888078-6B9C-4EF5-9096-604359987640}">
   <dimension ref="A1:V151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="86" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="142.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85.1796875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="51" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1862,10 +1954,9 @@
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -1875,24 +1966,25 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="11" t="s">
+        <v>299</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1902,23 +1994,21 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1926,47 +2016,43 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1979,22 +2065,24 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="21" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="16" t="s">
+        <v>300</v>
+      </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -2003,13 +2091,12 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -2022,10 +2109,9 @@
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
@@ -2033,20 +2119,18 @@
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -2056,10 +2140,9 @@
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
@@ -2067,10 +2150,9 @@
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -2079,10 +2161,9 @@
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -2092,21 +2173,19 @@
       <c r="A22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -2115,1983 +2194,1872 @@
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="11" t="s">
+        <v>303</v>
+      </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="25" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="23" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A26" s="4" t="s">
+      <c r="C25" s="11" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="A28" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="A29" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
+      <c r="C30" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A36" s="7" t="s">
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="13" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
+      <c r="D43" s="5"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
+      <c r="D44" s="5"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
+      <c r="D45" s="5"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
+      <c r="D46" s="5"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
+      <c r="D47" s="5"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
+      <c r="D50" s="5"/>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="11" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A53" s="9" t="s">
+      <c r="A53" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B53" s="11" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A54" s="9" t="s">
+      <c r="A54" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A55" s="9" t="s">
+      <c r="A55" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B55" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-    </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A56" s="9" t="s">
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+      <c r="A56" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="9"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A57" s="9" t="s">
+      <c r="A57" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="9"/>
-      <c r="K57" s="9"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
+      <c r="K57" s="5"/>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B58" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
-      <c r="H58" s="9"/>
-      <c r="I58" s="9"/>
-      <c r="J58" s="9"/>
-    </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A59" s="9" t="s">
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+    </row>
+    <row r="59" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A59" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="9"/>
-      <c r="I59" s="9"/>
-      <c r="J59" s="9"/>
-      <c r="K59" s="9"/>
-      <c r="L59" s="9"/>
-      <c r="M59" s="9"/>
-      <c r="N59" s="9"/>
-      <c r="O59" s="9"/>
-      <c r="P59" s="9"/>
-      <c r="Q59" s="9"/>
-      <c r="R59" s="9"/>
-      <c r="S59" s="9"/>
-      <c r="T59" s="9"/>
-      <c r="U59" s="9"/>
-      <c r="V59" s="9"/>
-    </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A60" s="9" t="s">
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="5"/>
+      <c r="O59" s="5"/>
+      <c r="P59" s="5"/>
+      <c r="Q59" s="5"/>
+      <c r="R59" s="5"/>
+      <c r="S59" s="5"/>
+      <c r="T59" s="5"/>
+      <c r="U59" s="5"/>
+      <c r="V59" s="5"/>
+    </row>
+    <row r="60" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+      <c r="A60" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B60" s="9" t="s">
+      <c r="B60" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
-      <c r="I60" s="9"/>
-      <c r="J60" s="9"/>
-      <c r="K60" s="9"/>
-      <c r="L60" s="9"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A61" s="9" t="s">
+      <c r="A61" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B61" s="9" t="s">
+      <c r="B61" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="9"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A62" s="9" t="s">
+      <c r="A62" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B62" s="9" t="s">
+      <c r="B62" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A63" s="9" t="s">
+      <c r="A63" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B63" s="9" t="s">
+      <c r="B63" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A64" s="9" t="s">
+      <c r="A64" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B64" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A65" s="9" t="s">
+      <c r="A65" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B65" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="C65" s="9"/>
-      <c r="D65" s="9"/>
-      <c r="E65" s="9"/>
-      <c r="F65" s="9"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A66" s="9" t="s">
+      <c r="A66" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="B66" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C66" s="9"/>
-      <c r="D66" s="9"/>
-      <c r="E66" s="9"/>
-      <c r="F66" s="9"/>
-      <c r="G66" s="9"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A67" s="9" t="s">
+      <c r="A67" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B67" s="9" t="s">
+      <c r="B67" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A68" s="9" t="s">
+      <c r="A68" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B68" s="9" t="s">
+      <c r="B68" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="C68" s="9"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A69" s="9" t="s">
+      <c r="A69" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="B69" s="9" t="s">
+      <c r="B69" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="C69" s="9"/>
-      <c r="D69" s="9"/>
-      <c r="E69" s="9"/>
-      <c r="F69" s="9"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A70" s="9" t="s">
+      <c r="A70" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B70" s="9" t="s">
+      <c r="B70" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="C70" s="9"/>
-      <c r="D70" s="9"/>
-      <c r="E70" s="9"/>
-      <c r="F70" s="9"/>
-      <c r="G70" s="9"/>
-      <c r="H70" s="9"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A71" s="9" t="s">
+      <c r="A71" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B71" s="9" t="s">
+      <c r="B71" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="C71" s="9"/>
-      <c r="D71" s="9"/>
-      <c r="E71" s="9"/>
-      <c r="F71" s="9"/>
-      <c r="G71" s="9"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A72" s="9" t="s">
+      <c r="A72" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B72" s="9" t="s">
+      <c r="B72" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="C72" s="9"/>
-      <c r="D72" s="9"/>
-      <c r="E72" s="9"/>
-      <c r="F72" s="9"/>
-      <c r="G72" s="9"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A73" s="9" t="s">
+      <c r="A73" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="B73" s="9" t="s">
+      <c r="B73" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="C73" s="9"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="9"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A74" s="9" t="s">
+      <c r="A74" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="B74" s="9" t="s">
+      <c r="B74" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="C74" s="9"/>
-      <c r="D74" s="9"/>
-      <c r="E74" s="9"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A75" s="12" t="s">
+      <c r="A75" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="B75" s="12" t="s">
+      <c r="B75" s="13" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A76" s="11" t="s">
+      <c r="A76" s="6" t="s">
         <v>148</v>
       </c>
       <c r="B76" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A77" s="11" t="s">
+      <c r="A77" s="6" t="s">
         <v>150</v>
       </c>
       <c r="B77" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="C77" s="11"/>
-      <c r="D77" s="11"/>
+      <c r="D77" s="6"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A78" s="11" t="s">
+      <c r="A78" s="6" t="s">
         <v>152</v>
       </c>
       <c r="B78" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="C78" s="11"/>
-      <c r="D78" s="11"/>
-      <c r="E78" s="11"/>
-      <c r="F78" s="11"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A79" s="11" t="s">
+      <c r="A79" s="6" t="s">
         <v>154</v>
       </c>
       <c r="B79" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="C79" s="11"/>
-      <c r="D79" s="11"/>
-      <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A80" s="11" t="s">
+      <c r="A80" s="6" t="s">
         <v>156</v>
       </c>
       <c r="B80" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="C80" s="11"/>
-      <c r="D80" s="11"/>
-      <c r="E80" s="11"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A81" s="11" t="s">
+      <c r="A81" s="6" t="s">
         <v>158</v>
       </c>
       <c r="B81" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="C81" s="11"/>
-      <c r="D81" s="11"/>
-      <c r="E81" s="11"/>
-      <c r="F81" s="11"/>
-      <c r="G81" s="11"/>
-      <c r="H81" s="11"/>
-      <c r="I81" s="11"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A82" s="11" t="s">
+      <c r="A82" s="6" t="s">
         <v>160</v>
       </c>
       <c r="B82" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="C82" s="11"/>
-      <c r="D82" s="11"/>
-      <c r="E82" s="11"/>
-      <c r="F82" s="11"/>
-      <c r="G82" s="11"/>
-      <c r="H82" s="11"/>
-      <c r="I82" s="11"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A83" s="11" t="s">
+      <c r="A83" s="6" t="s">
         <v>162</v>
       </c>
       <c r="B83" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C83" s="11"/>
-      <c r="D83" s="11"/>
-      <c r="E83" s="11"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A84" s="11" t="s">
+      <c r="A84" s="6" t="s">
         <v>164</v>
       </c>
       <c r="B84" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="C84" s="11"/>
-      <c r="D84" s="11"/>
-      <c r="E84" s="11"/>
-      <c r="F84" s="11"/>
-      <c r="G84" s="11"/>
-      <c r="H84" s="11"/>
-      <c r="I84" s="11"/>
-      <c r="J84" s="11"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
+      <c r="J84" s="6"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A85" s="11" t="s">
+      <c r="A85" s="6" t="s">
         <v>166</v>
       </c>
       <c r="B85" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="C85" s="11"/>
-      <c r="D85" s="11"/>
-      <c r="E85" s="11"/>
-      <c r="F85" s="11"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A86" s="11" t="s">
+      <c r="A86" s="6" t="s">
         <v>168</v>
       </c>
       <c r="B86" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="C86" s="11"/>
-      <c r="D86" s="11"/>
-      <c r="E86" s="11"/>
-      <c r="F86" s="11"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A87" s="11" t="s">
+      <c r="A87" s="6" t="s">
         <v>170</v>
       </c>
       <c r="B87" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="C87" s="11"/>
-      <c r="D87" s="11"/>
-      <c r="E87" s="11"/>
-      <c r="F87" s="11"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A88" s="11" t="s">
+      <c r="A88" s="6" t="s">
         <v>172</v>
       </c>
       <c r="B88" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="C88" s="11"/>
-      <c r="D88" s="11"/>
-      <c r="E88" s="11"/>
-      <c r="F88" s="11"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A89" s="11" t="s">
+      <c r="A89" s="6" t="s">
         <v>174</v>
       </c>
       <c r="B89" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="C89" s="11"/>
-      <c r="D89" s="11"/>
+      <c r="D89" s="6"/>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A90" s="11" t="s">
+      <c r="A90" s="6" t="s">
         <v>176</v>
       </c>
       <c r="B90" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="C90" s="11"/>
-      <c r="D90" s="11"/>
-      <c r="E90" s="11"/>
-      <c r="F90" s="11"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A91" s="11" t="s">
+      <c r="A91" s="6" t="s">
         <v>178</v>
       </c>
       <c r="B91" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="C91" s="11"/>
-      <c r="D91" s="11"/>
-      <c r="E91" s="11"/>
-      <c r="F91" s="11"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A92" s="11" t="s">
+      <c r="A92" s="6" t="s">
         <v>180</v>
       </c>
       <c r="B92" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="C92" s="11"/>
-      <c r="D92" s="11"/>
-      <c r="E92" s="11"/>
-      <c r="F92" s="11"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A93" s="11" t="s">
+      <c r="A93" s="6" t="s">
         <v>182</v>
       </c>
       <c r="B93" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="C93" s="11"/>
-      <c r="D93" s="11"/>
-      <c r="E93" s="11"/>
-      <c r="F93" s="11"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A94" s="11" t="s">
+      <c r="A94" s="6" t="s">
         <v>184</v>
       </c>
       <c r="B94" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="C94" s="11"/>
-      <c r="D94" s="11"/>
-      <c r="E94" s="11"/>
-      <c r="F94" s="11"/>
-      <c r="G94" s="11"/>
-      <c r="H94" s="11"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="6"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A95" s="11" t="s">
+      <c r="A95" s="6" t="s">
         <v>186</v>
       </c>
       <c r="B95" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="C95" s="11"/>
-      <c r="D95" s="11"/>
-      <c r="E95" s="11"/>
-      <c r="F95" s="11"/>
-      <c r="G95" s="11"/>
-      <c r="H95" s="11"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="6"/>
+      <c r="G95" s="6"/>
+      <c r="H95" s="6"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A96" s="11" t="s">
+      <c r="A96" s="6" t="s">
         <v>188</v>
       </c>
       <c r="B96" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="C96" s="11"/>
-      <c r="D96" s="11"/>
-      <c r="E96" s="11"/>
-      <c r="F96" s="11"/>
-      <c r="G96" s="11"/>
-      <c r="H96" s="11"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="6"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A97" s="11" t="s">
+      <c r="A97" s="6" t="s">
         <v>190</v>
       </c>
       <c r="B97" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="C97" s="11"/>
-      <c r="D97" s="11"/>
-      <c r="E97" s="11"/>
-      <c r="F97" s="11"/>
-      <c r="G97" s="11"/>
-      <c r="H97" s="11"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="6"/>
+      <c r="G97" s="6"/>
+      <c r="H97" s="6"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A98" s="11" t="s">
+      <c r="A98" s="6" t="s">
         <v>192</v>
       </c>
       <c r="B98" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
-      <c r="E98" s="11"/>
-      <c r="F98" s="11"/>
-      <c r="G98" s="11"/>
-      <c r="H98" s="11"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="6"/>
+      <c r="G98" s="6"/>
+      <c r="H98" s="6"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A99" s="11" t="s">
+      <c r="A99" s="6" t="s">
         <v>194</v>
       </c>
       <c r="B99" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="C99" s="11"/>
-      <c r="D99" s="11"/>
-      <c r="E99" s="11"/>
-      <c r="F99" s="11"/>
-      <c r="G99" s="11"/>
-      <c r="H99" s="11"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="6"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A100" s="11" t="s">
+      <c r="A100" s="6" t="s">
         <v>196</v>
       </c>
       <c r="B100" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="C100" s="11"/>
-      <c r="D100" s="11"/>
-      <c r="E100" s="11"/>
-      <c r="F100" s="11"/>
-      <c r="G100" s="11"/>
-      <c r="H100" s="11"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="6"/>
+      <c r="F100" s="6"/>
+      <c r="G100" s="6"/>
+      <c r="H100" s="6"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A101" s="11" t="s">
+      <c r="A101" s="6" t="s">
         <v>198</v>
       </c>
       <c r="B101" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="C101" s="11"/>
-      <c r="D101" s="11"/>
-      <c r="E101" s="11"/>
-      <c r="F101" s="11"/>
-      <c r="G101" s="11"/>
-      <c r="H101" s="11"/>
+      <c r="D101" s="6"/>
+      <c r="E101" s="6"/>
+      <c r="F101" s="6"/>
+      <c r="G101" s="6"/>
+      <c r="H101" s="6"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A102" s="11" t="s">
+      <c r="A102" s="6" t="s">
         <v>200</v>
       </c>
       <c r="B102" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="C102" s="11"/>
-      <c r="D102" s="11"/>
-      <c r="E102" s="11"/>
-      <c r="F102" s="11"/>
-      <c r="G102" s="11"/>
-      <c r="H102" s="11"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="6"/>
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A103" s="11" t="s">
+      <c r="A103" s="6" t="s">
         <v>202</v>
       </c>
       <c r="B103" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="C103" s="11"/>
-      <c r="D103" s="11"/>
-      <c r="E103" s="11"/>
-      <c r="F103" s="11"/>
-      <c r="G103" s="11"/>
-      <c r="H103" s="11"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="6"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A104" s="11" t="s">
+      <c r="A104" s="6" t="s">
         <v>204</v>
       </c>
       <c r="B104" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="C104" s="11"/>
-      <c r="D104" s="11"/>
-      <c r="E104" s="11"/>
-      <c r="F104" s="11"/>
-      <c r="G104" s="11"/>
-      <c r="H104" s="11"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="6"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="6"/>
+      <c r="H104" s="6"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A105" s="11" t="s">
+      <c r="A105" s="6" t="s">
         <v>206</v>
       </c>
       <c r="B105" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="C105" s="11"/>
-      <c r="D105" s="11"/>
-      <c r="E105" s="11"/>
-      <c r="F105" s="11"/>
-      <c r="G105" s="11"/>
-      <c r="H105" s="11"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="6"/>
+      <c r="F105" s="6"/>
+      <c r="G105" s="6"/>
+      <c r="H105" s="6"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A106" s="11" t="s">
+      <c r="A106" s="6" t="s">
         <v>208</v>
       </c>
       <c r="B106" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="C106" s="11"/>
-      <c r="D106" s="11"/>
-      <c r="E106" s="11"/>
-      <c r="F106" s="11"/>
-      <c r="G106" s="11"/>
-      <c r="H106" s="11"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="6"/>
+      <c r="F106" s="6"/>
+      <c r="G106" s="6"/>
+      <c r="H106" s="6"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A107" s="11" t="s">
+      <c r="A107" s="6" t="s">
         <v>210</v>
       </c>
       <c r="B107" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="C107" s="11"/>
-      <c r="D107" s="11"/>
-      <c r="E107" s="11"/>
-      <c r="F107" s="11"/>
-      <c r="G107" s="11"/>
-      <c r="H107" s="11"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="6"/>
+      <c r="F107" s="6"/>
+      <c r="G107" s="6"/>
+      <c r="H107" s="6"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A108" s="11" t="s">
+      <c r="A108" s="6" t="s">
         <v>212</v>
       </c>
       <c r="B108" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="C108" s="11"/>
-      <c r="D108" s="11"/>
-      <c r="E108" s="11"/>
-      <c r="F108" s="11"/>
-      <c r="G108" s="11"/>
+      <c r="D108" s="6"/>
+      <c r="E108" s="6"/>
+      <c r="F108" s="6"/>
+      <c r="G108" s="6"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A109" s="11" t="s">
+      <c r="A109" s="6" t="s">
         <v>214</v>
       </c>
       <c r="B109" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="C109" s="11"/>
-      <c r="D109" s="11"/>
-      <c r="E109" s="11"/>
-      <c r="F109" s="11"/>
-      <c r="G109" s="11"/>
+      <c r="D109" s="6"/>
+      <c r="E109" s="6"/>
+      <c r="F109" s="6"/>
+      <c r="G109" s="6"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A110" s="11" t="s">
+      <c r="A110" s="6" t="s">
         <v>216</v>
       </c>
       <c r="B110" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="C110" s="11"/>
-      <c r="D110" s="11"/>
-      <c r="E110" s="11"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="6"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A111" s="11" t="s">
+      <c r="A111" s="6" t="s">
         <v>218</v>
       </c>
       <c r="B111" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="C111" s="11"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A112" s="11" t="s">
+      <c r="A112" s="6" t="s">
         <v>220</v>
       </c>
       <c r="B112" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="C112" s="11"/>
-      <c r="D112" s="11"/>
+      <c r="D112" s="6"/>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A113" s="11" t="s">
+      <c r="A113" s="6" t="s">
         <v>222</v>
       </c>
       <c r="B113" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="C113" s="11"/>
-      <c r="D113" s="11"/>
-      <c r="E113" s="11"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="6"/>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A114" s="11" t="s">
+      <c r="A114" s="6" t="s">
         <v>224</v>
       </c>
       <c r="B114" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="C114" s="11"/>
-      <c r="D114" s="11"/>
-      <c r="E114" s="11"/>
+      <c r="D114" s="6"/>
+      <c r="E114" s="6"/>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A115" s="11" t="s">
+      <c r="A115" s="6" t="s">
         <v>226</v>
       </c>
       <c r="B115" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="C115" s="11"/>
-      <c r="D115" s="11"/>
-      <c r="E115" s="11"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A116" s="13" t="s">
+      <c r="A116" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="B116" s="13" t="s">
+      <c r="B116" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="C116" s="13"/>
-      <c r="D116" s="13"/>
-      <c r="E116" s="13"/>
-      <c r="F116" s="13"/>
-      <c r="G116" s="13"/>
-      <c r="H116" s="13"/>
-      <c r="I116" s="13"/>
+      <c r="D116" s="8"/>
+      <c r="E116" s="8"/>
+      <c r="F116" s="8"/>
+      <c r="G116" s="8"/>
+      <c r="H116" s="8"/>
+      <c r="I116" s="8"/>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A117" s="13" t="s">
+      <c r="A117" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="B117" s="13" t="s">
+      <c r="B117" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="C117" s="13"/>
-      <c r="D117" s="13"/>
-      <c r="E117" s="13"/>
-      <c r="F117" s="13"/>
-      <c r="G117" s="13"/>
-      <c r="H117" s="13"/>
-      <c r="I117" s="13"/>
-      <c r="J117" s="13"/>
-      <c r="K117" s="13"/>
-      <c r="L117" s="13"/>
-      <c r="M117" s="13"/>
-      <c r="N117" s="13"/>
-      <c r="O117" s="13"/>
-      <c r="P117" s="13"/>
-      <c r="Q117" s="13"/>
+      <c r="D117" s="8"/>
+      <c r="E117" s="8"/>
+      <c r="F117" s="8"/>
+      <c r="G117" s="8"/>
+      <c r="H117" s="8"/>
+      <c r="I117" s="8"/>
+      <c r="J117" s="8"/>
+      <c r="K117" s="8"/>
+      <c r="L117" s="8"/>
+      <c r="M117" s="8"/>
+      <c r="N117" s="8"/>
+      <c r="O117" s="8"/>
+      <c r="P117" s="8"/>
+      <c r="Q117" s="8"/>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A118" s="13" t="s">
+      <c r="A118" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="B118" s="13" t="s">
+      <c r="B118" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="C118" s="13"/>
-      <c r="D118" s="13"/>
-      <c r="E118" s="13"/>
-      <c r="F118" s="13"/>
-      <c r="G118" s="13"/>
-      <c r="H118" s="13"/>
-      <c r="I118" s="13"/>
-      <c r="J118" s="13"/>
-      <c r="K118" s="13"/>
-      <c r="L118" s="13"/>
-      <c r="M118" s="13"/>
-      <c r="N118" s="13"/>
-      <c r="O118" s="13"/>
-      <c r="P118" s="13"/>
-      <c r="Q118" s="13"/>
+      <c r="D118" s="8"/>
+      <c r="E118" s="8"/>
+      <c r="F118" s="8"/>
+      <c r="G118" s="8"/>
+      <c r="H118" s="8"/>
+      <c r="I118" s="8"/>
+      <c r="J118" s="8"/>
+      <c r="K118" s="8"/>
+      <c r="L118" s="8"/>
+      <c r="M118" s="8"/>
+      <c r="N118" s="8"/>
+      <c r="O118" s="8"/>
+      <c r="P118" s="8"/>
+      <c r="Q118" s="8"/>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A119" s="13" t="s">
+      <c r="A119" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="B119" s="13" t="s">
+      <c r="B119" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="C119" s="13"/>
-      <c r="D119" s="13"/>
-      <c r="E119" s="13"/>
-      <c r="F119" s="13"/>
-      <c r="G119" s="13"/>
-      <c r="H119" s="13"/>
-      <c r="I119" s="13"/>
-      <c r="J119" s="13"/>
-      <c r="K119" s="13"/>
-      <c r="L119" s="13"/>
-      <c r="M119" s="13"/>
-      <c r="N119" s="13"/>
-      <c r="O119" s="13"/>
-      <c r="P119" s="13"/>
-      <c r="Q119" s="13"/>
+      <c r="D119" s="8"/>
+      <c r="E119" s="8"/>
+      <c r="F119" s="8"/>
+      <c r="G119" s="8"/>
+      <c r="H119" s="8"/>
+      <c r="I119" s="8"/>
+      <c r="J119" s="8"/>
+      <c r="K119" s="8"/>
+      <c r="L119" s="8"/>
+      <c r="M119" s="8"/>
+      <c r="N119" s="8"/>
+      <c r="O119" s="8"/>
+      <c r="P119" s="8"/>
+      <c r="Q119" s="8"/>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A120" s="13" t="s">
+      <c r="A120" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="B120" s="13" t="s">
+      <c r="B120" s="20" t="s">
         <v>237</v>
       </c>
-      <c r="C120" s="13"/>
-      <c r="D120" s="13"/>
-      <c r="E120" s="13"/>
-      <c r="F120" s="13"/>
-      <c r="G120" s="13"/>
-      <c r="H120" s="13"/>
-      <c r="I120" s="13"/>
-      <c r="J120" s="13"/>
-      <c r="K120" s="13"/>
-      <c r="L120" s="13"/>
-      <c r="M120" s="13"/>
-      <c r="N120" s="13"/>
-      <c r="O120" s="13"/>
-      <c r="P120" s="13"/>
-      <c r="Q120" s="13"/>
+      <c r="D120" s="8"/>
+      <c r="E120" s="8"/>
+      <c r="F120" s="8"/>
+      <c r="G120" s="8"/>
+      <c r="H120" s="8"/>
+      <c r="I120" s="8"/>
+      <c r="J120" s="8"/>
+      <c r="K120" s="8"/>
+      <c r="L120" s="8"/>
+      <c r="M120" s="8"/>
+      <c r="N120" s="8"/>
+      <c r="O120" s="8"/>
+      <c r="P120" s="8"/>
+      <c r="Q120" s="8"/>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A121" s="13" t="s">
+      <c r="A121" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="B121" s="13" t="s">
+      <c r="B121" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="C121" s="13"/>
-      <c r="D121" s="13"/>
-      <c r="E121" s="13"/>
-      <c r="F121" s="13"/>
-      <c r="G121" s="13"/>
-      <c r="H121" s="13"/>
-      <c r="I121" s="13"/>
-      <c r="J121" s="13"/>
-      <c r="K121" s="13"/>
-      <c r="L121" s="13"/>
-      <c r="M121" s="13"/>
-      <c r="N121" s="13"/>
-      <c r="O121" s="13"/>
-      <c r="P121" s="13"/>
-      <c r="Q121" s="13"/>
+      <c r="D121" s="8"/>
+      <c r="E121" s="8"/>
+      <c r="F121" s="8"/>
+      <c r="G121" s="8"/>
+      <c r="H121" s="8"/>
+      <c r="I121" s="8"/>
+      <c r="J121" s="8"/>
+      <c r="K121" s="8"/>
+      <c r="L121" s="8"/>
+      <c r="M121" s="8"/>
+      <c r="N121" s="8"/>
+      <c r="O121" s="8"/>
+      <c r="P121" s="8"/>
+      <c r="Q121" s="8"/>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A122" s="13" t="s">
+      <c r="A122" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="B122" s="13" t="s">
+      <c r="B122" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="C122" s="13"/>
-      <c r="D122" s="13"/>
-      <c r="E122" s="13"/>
-      <c r="F122" s="13"/>
-      <c r="G122" s="13"/>
-      <c r="H122" s="13"/>
-      <c r="I122" s="13"/>
-      <c r="J122" s="13"/>
-      <c r="K122" s="13"/>
-      <c r="L122" s="13"/>
-      <c r="M122" s="13"/>
-      <c r="N122" s="13"/>
-      <c r="O122" s="13"/>
-      <c r="P122" s="13"/>
-      <c r="Q122" s="13"/>
+      <c r="D122" s="8"/>
+      <c r="E122" s="8"/>
+      <c r="F122" s="8"/>
+      <c r="G122" s="8"/>
+      <c r="H122" s="8"/>
+      <c r="I122" s="8"/>
+      <c r="J122" s="8"/>
+      <c r="K122" s="8"/>
+      <c r="L122" s="8"/>
+      <c r="M122" s="8"/>
+      <c r="N122" s="8"/>
+      <c r="O122" s="8"/>
+      <c r="P122" s="8"/>
+      <c r="Q122" s="8"/>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A123" s="13" t="s">
+      <c r="A123" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="B123" s="13" t="s">
+      <c r="B123" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="C123" s="13"/>
-      <c r="D123" s="13"/>
-      <c r="E123" s="13"/>
-      <c r="F123" s="13"/>
-      <c r="G123" s="13"/>
-      <c r="H123" s="13"/>
-      <c r="I123" s="13"/>
-      <c r="J123" s="13"/>
-      <c r="K123" s="13"/>
-      <c r="L123" s="13"/>
-      <c r="M123" s="13"/>
-      <c r="N123" s="13"/>
-      <c r="O123" s="13"/>
-      <c r="P123" s="13"/>
-      <c r="Q123" s="13"/>
+      <c r="D123" s="8"/>
+      <c r="E123" s="8"/>
+      <c r="F123" s="8"/>
+      <c r="G123" s="8"/>
+      <c r="H123" s="8"/>
+      <c r="I123" s="8"/>
+      <c r="J123" s="8"/>
+      <c r="K123" s="8"/>
+      <c r="L123" s="8"/>
+      <c r="M123" s="8"/>
+      <c r="N123" s="8"/>
+      <c r="O123" s="8"/>
+      <c r="P123" s="8"/>
+      <c r="Q123" s="8"/>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A124" s="13" t="s">
+      <c r="A124" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="B124" s="13" t="s">
+      <c r="B124" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="C124" s="13"/>
-      <c r="D124" s="13"/>
-      <c r="E124" s="13"/>
-      <c r="F124" s="13"/>
-      <c r="G124" s="13"/>
-      <c r="H124" s="13"/>
-      <c r="I124" s="13"/>
-      <c r="J124" s="13"/>
-      <c r="K124" s="13"/>
-      <c r="L124" s="13"/>
-      <c r="M124" s="13"/>
-      <c r="N124" s="13"/>
-      <c r="O124" s="13"/>
-      <c r="P124" s="13"/>
-      <c r="Q124" s="13"/>
+      <c r="D124" s="8"/>
+      <c r="E124" s="8"/>
+      <c r="F124" s="8"/>
+      <c r="G124" s="8"/>
+      <c r="H124" s="8"/>
+      <c r="I124" s="8"/>
+      <c r="J124" s="8"/>
+      <c r="K124" s="8"/>
+      <c r="L124" s="8"/>
+      <c r="M124" s="8"/>
+      <c r="N124" s="8"/>
+      <c r="O124" s="8"/>
+      <c r="P124" s="8"/>
+      <c r="Q124" s="8"/>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A125" s="13" t="s">
+      <c r="A125" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="B125" s="13" t="s">
+      <c r="B125" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="C125" s="13"/>
-      <c r="D125" s="13"/>
-      <c r="E125" s="13"/>
-      <c r="F125" s="13"/>
-      <c r="G125" s="13"/>
-      <c r="H125" s="13"/>
-      <c r="I125" s="13"/>
-      <c r="J125" s="13"/>
-      <c r="K125" s="13"/>
-      <c r="L125" s="13"/>
-      <c r="M125" s="13"/>
-      <c r="N125" s="13"/>
-      <c r="O125" s="13"/>
-      <c r="P125" s="13"/>
-      <c r="Q125" s="13"/>
+      <c r="D125" s="8"/>
+      <c r="E125" s="8"/>
+      <c r="F125" s="8"/>
+      <c r="G125" s="8"/>
+      <c r="H125" s="8"/>
+      <c r="I125" s="8"/>
+      <c r="J125" s="8"/>
+      <c r="K125" s="8"/>
+      <c r="L125" s="8"/>
+      <c r="M125" s="8"/>
+      <c r="N125" s="8"/>
+      <c r="O125" s="8"/>
+      <c r="P125" s="8"/>
+      <c r="Q125" s="8"/>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A126" s="13" t="s">
+      <c r="A126" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="B126" s="13" t="s">
+      <c r="B126" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="C126" s="13"/>
-      <c r="D126" s="13"/>
-      <c r="E126" s="13"/>
-      <c r="F126" s="13"/>
-      <c r="G126" s="13"/>
-      <c r="H126" s="13"/>
-      <c r="I126" s="13"/>
-      <c r="J126" s="13"/>
-      <c r="K126" s="13"/>
-      <c r="L126" s="13"/>
-      <c r="M126" s="13"/>
-      <c r="N126" s="13"/>
-      <c r="O126" s="13"/>
-      <c r="P126" s="13"/>
-      <c r="Q126" s="13"/>
-    </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A127" s="13" t="s">
+      <c r="D126" s="8"/>
+      <c r="E126" s="8"/>
+      <c r="F126" s="8"/>
+      <c r="G126" s="8"/>
+      <c r="H126" s="8"/>
+      <c r="I126" s="8"/>
+      <c r="J126" s="8"/>
+      <c r="K126" s="8"/>
+      <c r="L126" s="8"/>
+      <c r="M126" s="8"/>
+      <c r="N126" s="8"/>
+      <c r="O126" s="8"/>
+      <c r="P126" s="8"/>
+      <c r="Q126" s="8"/>
+    </row>
+    <row r="127" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="A127" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B127" s="13" t="s">
+      <c r="B127" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="C127" s="13"/>
-      <c r="D127" s="13"/>
-      <c r="E127" s="13"/>
-      <c r="F127" s="13"/>
-      <c r="G127" s="13"/>
-      <c r="H127" s="13"/>
-      <c r="I127" s="13"/>
-      <c r="J127" s="13"/>
-      <c r="K127" s="13"/>
-      <c r="L127" s="13"/>
-      <c r="M127" s="13"/>
-      <c r="N127" s="13"/>
-      <c r="O127" s="13"/>
-      <c r="P127" s="13"/>
-      <c r="Q127" s="13"/>
+      <c r="D127" s="8"/>
+      <c r="E127" s="8"/>
+      <c r="F127" s="8"/>
+      <c r="G127" s="8"/>
+      <c r="H127" s="8"/>
+      <c r="I127" s="8"/>
+      <c r="J127" s="8"/>
+      <c r="K127" s="8"/>
+      <c r="L127" s="8"/>
+      <c r="M127" s="8"/>
+      <c r="N127" s="8"/>
+      <c r="O127" s="8"/>
+      <c r="P127" s="8"/>
+      <c r="Q127" s="8"/>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A128" s="13" t="s">
+      <c r="A128" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="B128" s="13" t="s">
+      <c r="B128" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="C128" s="13"/>
-      <c r="D128" s="13"/>
-      <c r="E128" s="13"/>
-      <c r="F128" s="13"/>
-      <c r="G128" s="13"/>
-      <c r="H128" s="13"/>
-      <c r="I128" s="13"/>
-      <c r="J128" s="13"/>
-      <c r="K128" s="13"/>
-      <c r="L128" s="13"/>
-      <c r="M128" s="13"/>
-      <c r="N128" s="13"/>
-      <c r="O128" s="13"/>
-      <c r="P128" s="13"/>
-      <c r="Q128" s="13"/>
+      <c r="D128" s="8"/>
+      <c r="E128" s="8"/>
+      <c r="F128" s="8"/>
+      <c r="G128" s="8"/>
+      <c r="H128" s="8"/>
+      <c r="I128" s="8"/>
+      <c r="J128" s="8"/>
+      <c r="K128" s="8"/>
+      <c r="L128" s="8"/>
+      <c r="M128" s="8"/>
+      <c r="N128" s="8"/>
+      <c r="O128" s="8"/>
+      <c r="P128" s="8"/>
+      <c r="Q128" s="8"/>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A129" s="13" t="s">
+      <c r="A129" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="B129" s="13" t="s">
+      <c r="B129" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="C129" s="13"/>
-      <c r="D129" s="13"/>
-      <c r="E129" s="13"/>
-      <c r="F129" s="13"/>
-      <c r="G129" s="13"/>
-      <c r="H129" s="13"/>
-      <c r="I129" s="13"/>
-      <c r="J129" s="13"/>
-      <c r="K129" s="13"/>
-      <c r="L129" s="13"/>
-      <c r="M129" s="13"/>
-      <c r="N129" s="13"/>
-      <c r="O129" s="13"/>
-      <c r="P129" s="13"/>
-      <c r="Q129" s="13"/>
+      <c r="D129" s="8"/>
+      <c r="E129" s="8"/>
+      <c r="F129" s="8"/>
+      <c r="G129" s="8"/>
+      <c r="H129" s="8"/>
+      <c r="I129" s="8"/>
+      <c r="J129" s="8"/>
+      <c r="K129" s="8"/>
+      <c r="L129" s="8"/>
+      <c r="M129" s="8"/>
+      <c r="N129" s="8"/>
+      <c r="O129" s="8"/>
+      <c r="P129" s="8"/>
+      <c r="Q129" s="8"/>
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A130" s="13" t="s">
+      <c r="A130" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="B130" s="13" t="s">
+      <c r="B130" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="C130" s="13"/>
-      <c r="D130" s="13"/>
-      <c r="E130" s="13"/>
-      <c r="F130" s="13"/>
-      <c r="G130" s="13"/>
-      <c r="H130" s="13"/>
-      <c r="I130" s="13"/>
-      <c r="J130" s="13"/>
-      <c r="K130" s="13"/>
-      <c r="L130" s="13"/>
-      <c r="M130" s="13"/>
-      <c r="N130" s="13"/>
-      <c r="O130" s="13"/>
-      <c r="P130" s="13"/>
-      <c r="Q130" s="13"/>
+      <c r="D130" s="8"/>
+      <c r="E130" s="8"/>
+      <c r="F130" s="8"/>
+      <c r="G130" s="8"/>
+      <c r="H130" s="8"/>
+      <c r="I130" s="8"/>
+      <c r="J130" s="8"/>
+      <c r="K130" s="8"/>
+      <c r="L130" s="8"/>
+      <c r="M130" s="8"/>
+      <c r="N130" s="8"/>
+      <c r="O130" s="8"/>
+      <c r="P130" s="8"/>
+      <c r="Q130" s="8"/>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A131" s="13" t="s">
+      <c r="A131" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="B131" s="13" t="s">
+      <c r="B131" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="C131" s="13"/>
-      <c r="D131" s="13"/>
-      <c r="E131" s="13"/>
-      <c r="F131" s="13"/>
-      <c r="G131" s="13"/>
-      <c r="H131" s="13"/>
-      <c r="I131" s="13"/>
-      <c r="J131" s="13"/>
-      <c r="K131" s="13"/>
-      <c r="L131" s="13"/>
-      <c r="M131" s="13"/>
-      <c r="N131" s="13"/>
-      <c r="O131" s="13"/>
-      <c r="P131" s="13"/>
-      <c r="Q131" s="13"/>
+      <c r="D131" s="8"/>
+      <c r="E131" s="8"/>
+      <c r="F131" s="8"/>
+      <c r="G131" s="8"/>
+      <c r="H131" s="8"/>
+      <c r="I131" s="8"/>
+      <c r="J131" s="8"/>
+      <c r="K131" s="8"/>
+      <c r="L131" s="8"/>
+      <c r="M131" s="8"/>
+      <c r="N131" s="8"/>
+      <c r="O131" s="8"/>
+      <c r="P131" s="8"/>
+      <c r="Q131" s="8"/>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A132" s="13" t="s">
+      <c r="A132" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B132" s="13" t="s">
+      <c r="B132" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="C132" s="13"/>
-      <c r="D132" s="13"/>
-      <c r="E132" s="13"/>
-      <c r="F132" s="13"/>
-      <c r="G132" s="13"/>
-      <c r="H132" s="13"/>
-      <c r="I132" s="13"/>
-      <c r="J132" s="13"/>
-      <c r="K132" s="13"/>
-      <c r="L132" s="13"/>
-      <c r="M132" s="13"/>
-      <c r="N132" s="13"/>
-      <c r="O132" s="13"/>
-      <c r="P132" s="13"/>
-      <c r="Q132" s="13"/>
-    </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A133" s="13" t="s">
+      <c r="D132" s="8"/>
+      <c r="E132" s="8"/>
+      <c r="F132" s="8"/>
+      <c r="G132" s="8"/>
+      <c r="H132" s="8"/>
+      <c r="I132" s="8"/>
+      <c r="J132" s="8"/>
+      <c r="K132" s="8"/>
+      <c r="L132" s="8"/>
+      <c r="M132" s="8"/>
+      <c r="N132" s="8"/>
+      <c r="O132" s="8"/>
+      <c r="P132" s="8"/>
+      <c r="Q132" s="8"/>
+    </row>
+    <row r="133" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="A133" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="B133" s="13" t="s">
+      <c r="B133" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="C133" s="13"/>
-      <c r="D133" s="13"/>
-      <c r="E133" s="13"/>
-      <c r="F133" s="13"/>
-      <c r="G133" s="13"/>
-      <c r="H133" s="13"/>
-      <c r="I133" s="13"/>
-      <c r="J133" s="13"/>
-      <c r="K133" s="13"/>
-      <c r="L133" s="13"/>
-      <c r="M133" s="13"/>
-      <c r="N133" s="13"/>
-      <c r="O133" s="13"/>
-      <c r="P133" s="13"/>
-      <c r="Q133" s="13"/>
-    </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A134" s="13" t="s">
+      <c r="D133" s="8"/>
+      <c r="E133" s="8"/>
+      <c r="F133" s="8"/>
+      <c r="G133" s="8"/>
+      <c r="H133" s="8"/>
+      <c r="I133" s="8"/>
+      <c r="J133" s="8"/>
+      <c r="K133" s="8"/>
+      <c r="L133" s="8"/>
+      <c r="M133" s="8"/>
+      <c r="N133" s="8"/>
+      <c r="O133" s="8"/>
+      <c r="P133" s="8"/>
+      <c r="Q133" s="8"/>
+    </row>
+    <row r="134" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="A134" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="B134" s="13" t="s">
+      <c r="B134" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="C134" s="13"/>
-      <c r="D134" s="13"/>
-      <c r="E134" s="13"/>
-      <c r="F134" s="13"/>
-      <c r="G134" s="13"/>
-      <c r="H134" s="13"/>
-      <c r="I134" s="13"/>
-      <c r="J134" s="13"/>
-      <c r="K134" s="13"/>
-      <c r="L134" s="13"/>
-      <c r="M134" s="13"/>
-      <c r="N134" s="13"/>
-      <c r="O134" s="13"/>
-      <c r="P134" s="13"/>
-      <c r="Q134" s="13"/>
+      <c r="D134" s="8"/>
+      <c r="E134" s="8"/>
+      <c r="F134" s="8"/>
+      <c r="G134" s="8"/>
+      <c r="H134" s="8"/>
+      <c r="I134" s="8"/>
+      <c r="J134" s="8"/>
+      <c r="K134" s="8"/>
+      <c r="L134" s="8"/>
+      <c r="M134" s="8"/>
+      <c r="N134" s="8"/>
+      <c r="O134" s="8"/>
+      <c r="P134" s="8"/>
+      <c r="Q134" s="8"/>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A135" s="13" t="s">
+      <c r="A135" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="B135" s="13" t="s">
+      <c r="B135" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="C135" s="13"/>
-      <c r="D135" s="13"/>
-      <c r="E135" s="13"/>
-      <c r="F135" s="13"/>
-      <c r="G135" s="13"/>
-      <c r="H135" s="13"/>
-      <c r="I135" s="13"/>
-      <c r="J135" s="13"/>
-      <c r="K135" s="13"/>
-      <c r="L135" s="13"/>
-      <c r="M135" s="13"/>
-      <c r="N135" s="13"/>
-      <c r="O135" s="13"/>
-      <c r="P135" s="13"/>
-      <c r="Q135" s="13"/>
+      <c r="D135" s="8"/>
+      <c r="E135" s="8"/>
+      <c r="F135" s="8"/>
+      <c r="G135" s="8"/>
+      <c r="H135" s="8"/>
+      <c r="I135" s="8"/>
+      <c r="J135" s="8"/>
+      <c r="K135" s="8"/>
+      <c r="L135" s="8"/>
+      <c r="M135" s="8"/>
+      <c r="N135" s="8"/>
+      <c r="O135" s="8"/>
+      <c r="P135" s="8"/>
+      <c r="Q135" s="8"/>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A136" s="13" t="s">
+      <c r="A136" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="B136" s="13" t="s">
+      <c r="B136" s="11" t="s">
         <v>269</v>
       </c>
-      <c r="C136" s="13"/>
-      <c r="D136" s="13"/>
-      <c r="E136" s="13"/>
-      <c r="F136" s="13"/>
-      <c r="G136" s="13"/>
-      <c r="H136" s="13"/>
-      <c r="I136" s="13"/>
-      <c r="J136" s="13"/>
-      <c r="K136" s="13"/>
-      <c r="L136" s="13"/>
-      <c r="M136" s="13"/>
-      <c r="N136" s="13"/>
-      <c r="O136" s="13"/>
-      <c r="P136" s="13"/>
-      <c r="Q136" s="13"/>
-    </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A137" s="13" t="s">
+      <c r="D136" s="8"/>
+      <c r="E136" s="8"/>
+      <c r="F136" s="8"/>
+      <c r="G136" s="8"/>
+      <c r="H136" s="8"/>
+      <c r="I136" s="8"/>
+      <c r="J136" s="8"/>
+      <c r="K136" s="8"/>
+      <c r="L136" s="8"/>
+      <c r="M136" s="8"/>
+      <c r="N136" s="8"/>
+      <c r="O136" s="8"/>
+      <c r="P136" s="8"/>
+      <c r="Q136" s="8"/>
+    </row>
+    <row r="137" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A137" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="B137" s="13" t="s">
+      <c r="B137" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="C137" s="13"/>
-      <c r="D137" s="13"/>
-      <c r="E137" s="13"/>
-      <c r="F137" s="13"/>
-      <c r="G137" s="13"/>
-      <c r="H137" s="13"/>
-      <c r="I137" s="13"/>
-      <c r="J137" s="13"/>
-      <c r="K137" s="13"/>
-      <c r="L137" s="13"/>
-      <c r="M137" s="13"/>
-      <c r="N137" s="13"/>
-      <c r="O137" s="13"/>
-      <c r="P137" s="13"/>
-      <c r="Q137" s="13"/>
-    </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A138" s="13" t="s">
+      <c r="D137" s="8"/>
+      <c r="E137" s="8"/>
+      <c r="F137" s="8"/>
+      <c r="G137" s="8"/>
+      <c r="H137" s="8"/>
+      <c r="I137" s="8"/>
+      <c r="J137" s="8"/>
+      <c r="K137" s="8"/>
+      <c r="L137" s="8"/>
+      <c r="M137" s="8"/>
+      <c r="N137" s="8"/>
+      <c r="O137" s="8"/>
+      <c r="P137" s="8"/>
+      <c r="Q137" s="8"/>
+    </row>
+    <row r="138" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="A138" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="B138" s="13" t="s">
+      <c r="B138" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="C138" s="13"/>
-      <c r="D138" s="13"/>
-      <c r="E138" s="13"/>
-      <c r="F138" s="13"/>
-      <c r="G138" s="13"/>
-      <c r="H138" s="13"/>
-      <c r="I138" s="13"/>
-      <c r="J138" s="13"/>
-      <c r="K138" s="13"/>
-      <c r="L138" s="13"/>
-      <c r="M138" s="13"/>
-      <c r="N138" s="13"/>
-      <c r="O138" s="13"/>
-      <c r="P138" s="13"/>
-      <c r="Q138" s="13"/>
+      <c r="D138" s="8"/>
+      <c r="E138" s="8"/>
+      <c r="F138" s="8"/>
+      <c r="G138" s="8"/>
+      <c r="H138" s="8"/>
+      <c r="I138" s="8"/>
+      <c r="J138" s="8"/>
+      <c r="K138" s="8"/>
+      <c r="L138" s="8"/>
+      <c r="M138" s="8"/>
+      <c r="N138" s="8"/>
+      <c r="O138" s="8"/>
+      <c r="P138" s="8"/>
+      <c r="Q138" s="8"/>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A139" s="13" t="s">
+      <c r="A139" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="B139" s="13" t="s">
+      <c r="B139" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="C139" s="13"/>
-      <c r="D139" s="13"/>
-      <c r="E139" s="13"/>
-      <c r="F139" s="13"/>
-      <c r="G139" s="13"/>
-      <c r="H139" s="13"/>
-      <c r="I139" s="13"/>
-      <c r="J139" s="13"/>
-      <c r="K139" s="13"/>
-      <c r="L139" s="13"/>
-      <c r="M139" s="13"/>
-      <c r="N139" s="13"/>
-      <c r="O139" s="13"/>
-      <c r="P139" s="13"/>
-      <c r="Q139" s="13"/>
+      <c r="D139" s="8"/>
+      <c r="E139" s="8"/>
+      <c r="F139" s="8"/>
+      <c r="G139" s="8"/>
+      <c r="H139" s="8"/>
+      <c r="I139" s="8"/>
+      <c r="J139" s="8"/>
+      <c r="K139" s="8"/>
+      <c r="L139" s="8"/>
+      <c r="M139" s="8"/>
+      <c r="N139" s="8"/>
+      <c r="O139" s="8"/>
+      <c r="P139" s="8"/>
+      <c r="Q139" s="8"/>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A140" s="13" t="s">
+      <c r="A140" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="B140" s="13" t="s">
+      <c r="B140" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="C140" s="13"/>
-      <c r="D140" s="13"/>
-      <c r="E140" s="13"/>
-      <c r="F140" s="13"/>
-      <c r="G140" s="13"/>
-      <c r="H140" s="13"/>
-      <c r="I140" s="13"/>
-      <c r="J140" s="13"/>
-      <c r="K140" s="13"/>
-      <c r="L140" s="13"/>
-      <c r="M140" s="13"/>
-      <c r="N140" s="13"/>
-      <c r="O140" s="13"/>
-      <c r="P140" s="13"/>
-      <c r="Q140" s="13"/>
-    </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A141" s="13" t="s">
+      <c r="D140" s="8"/>
+      <c r="E140" s="8"/>
+      <c r="F140" s="8"/>
+      <c r="G140" s="8"/>
+      <c r="H140" s="8"/>
+      <c r="I140" s="8"/>
+      <c r="J140" s="8"/>
+      <c r="K140" s="8"/>
+      <c r="L140" s="8"/>
+      <c r="M140" s="8"/>
+      <c r="N140" s="8"/>
+      <c r="O140" s="8"/>
+      <c r="P140" s="8"/>
+      <c r="Q140" s="8"/>
+    </row>
+    <row r="141" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A141" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="B141" s="13" t="s">
+      <c r="B141" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="C141" s="13"/>
-      <c r="D141" s="13"/>
-      <c r="E141" s="13"/>
-      <c r="F141" s="13"/>
-      <c r="G141" s="13"/>
-      <c r="H141" s="13"/>
-      <c r="I141" s="13"/>
-      <c r="J141" s="13"/>
-      <c r="K141" s="13"/>
-      <c r="L141" s="13"/>
-      <c r="M141" s="13"/>
-      <c r="N141" s="13"/>
-      <c r="O141" s="13"/>
-      <c r="P141" s="13"/>
-      <c r="Q141" s="13"/>
+      <c r="D141" s="8"/>
+      <c r="E141" s="8"/>
+      <c r="F141" s="8"/>
+      <c r="G141" s="8"/>
+      <c r="H141" s="8"/>
+      <c r="I141" s="8"/>
+      <c r="J141" s="8"/>
+      <c r="K141" s="8"/>
+      <c r="L141" s="8"/>
+      <c r="M141" s="8"/>
+      <c r="N141" s="8"/>
+      <c r="O141" s="8"/>
+      <c r="P141" s="8"/>
+      <c r="Q141" s="8"/>
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A142" s="13" t="s">
+      <c r="A142" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="B142" s="13" t="s">
+      <c r="B142" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="C142" s="13"/>
-      <c r="D142" s="13"/>
-      <c r="E142" s="13"/>
-      <c r="F142" s="13"/>
-      <c r="G142" s="13"/>
-      <c r="H142" s="13"/>
-      <c r="I142" s="13"/>
-      <c r="J142" s="13"/>
-      <c r="K142" s="13"/>
-      <c r="L142" s="13"/>
-      <c r="M142" s="13"/>
-      <c r="N142" s="13"/>
-      <c r="O142" s="13"/>
-      <c r="P142" s="13"/>
-      <c r="Q142" s="13"/>
+      <c r="D142" s="8"/>
+      <c r="E142" s="8"/>
+      <c r="F142" s="8"/>
+      <c r="G142" s="8"/>
+      <c r="H142" s="8"/>
+      <c r="I142" s="8"/>
+      <c r="J142" s="8"/>
+      <c r="K142" s="8"/>
+      <c r="L142" s="8"/>
+      <c r="M142" s="8"/>
+      <c r="N142" s="8"/>
+      <c r="O142" s="8"/>
+      <c r="P142" s="8"/>
+      <c r="Q142" s="8"/>
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A143" s="13" t="s">
+      <c r="A143" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="B143" s="13" t="s">
+      <c r="B143" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="C143" s="13"/>
-      <c r="D143" s="13"/>
-      <c r="E143" s="13"/>
-      <c r="F143" s="13"/>
-      <c r="G143" s="13"/>
-      <c r="H143" s="13"/>
-      <c r="I143" s="13"/>
-      <c r="J143" s="13"/>
-      <c r="K143" s="13"/>
-      <c r="L143" s="13"/>
-      <c r="M143" s="13"/>
-      <c r="N143" s="13"/>
-      <c r="O143" s="13"/>
-      <c r="P143" s="13"/>
-      <c r="Q143" s="13"/>
+      <c r="D143" s="8"/>
+      <c r="E143" s="8"/>
+      <c r="F143" s="8"/>
+      <c r="G143" s="8"/>
+      <c r="H143" s="8"/>
+      <c r="I143" s="8"/>
+      <c r="J143" s="8"/>
+      <c r="K143" s="8"/>
+      <c r="L143" s="8"/>
+      <c r="M143" s="8"/>
+      <c r="N143" s="8"/>
+      <c r="O143" s="8"/>
+      <c r="P143" s="8"/>
+      <c r="Q143" s="8"/>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A144" s="13" t="s">
+      <c r="A144" s="19" t="s">
         <v>284</v>
       </c>
-      <c r="B144" s="13" t="s">
+      <c r="B144" s="20" t="s">
         <v>285</v>
       </c>
-      <c r="C144" s="13"/>
-      <c r="D144" s="13"/>
-      <c r="E144" s="13"/>
-      <c r="F144" s="13"/>
-      <c r="G144" s="13"/>
-      <c r="H144" s="13"/>
-      <c r="I144" s="13"/>
-      <c r="J144" s="13"/>
-      <c r="K144" s="13"/>
-      <c r="L144" s="13"/>
-      <c r="M144" s="13"/>
-      <c r="N144" s="13"/>
-      <c r="O144" s="13"/>
-      <c r="P144" s="13"/>
-      <c r="Q144" s="13"/>
-    </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A145" s="13" t="s">
+      <c r="D144" s="8"/>
+      <c r="E144" s="8"/>
+      <c r="F144" s="8"/>
+      <c r="G144" s="8"/>
+      <c r="H144" s="8"/>
+      <c r="I144" s="8"/>
+      <c r="J144" s="8"/>
+      <c r="K144" s="8"/>
+      <c r="L144" s="8"/>
+      <c r="M144" s="8"/>
+      <c r="N144" s="8"/>
+      <c r="O144" s="8"/>
+      <c r="P144" s="8"/>
+      <c r="Q144" s="8"/>
+    </row>
+    <row r="145" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="A145" s="19" t="s">
         <v>286</v>
       </c>
-      <c r="B145" s="13" t="s">
+      <c r="B145" s="20" t="s">
         <v>287</v>
       </c>
-      <c r="C145" s="13"/>
-      <c r="D145" s="13"/>
-      <c r="E145" s="13"/>
-      <c r="F145" s="13"/>
-      <c r="G145" s="13"/>
-      <c r="H145" s="13"/>
-      <c r="I145" s="13"/>
-      <c r="J145" s="13"/>
-      <c r="K145" s="13"/>
-      <c r="L145" s="13"/>
-      <c r="M145" s="13"/>
-      <c r="N145" s="13"/>
-      <c r="O145" s="13"/>
-      <c r="P145" s="13"/>
-      <c r="Q145" s="13"/>
+      <c r="D145" s="8"/>
+      <c r="E145" s="8"/>
+      <c r="F145" s="8"/>
+      <c r="G145" s="8"/>
+      <c r="H145" s="8"/>
+      <c r="I145" s="8"/>
+      <c r="J145" s="8"/>
+      <c r="K145" s="8"/>
+      <c r="L145" s="8"/>
+      <c r="M145" s="8"/>
+      <c r="N145" s="8"/>
+      <c r="O145" s="8"/>
+      <c r="P145" s="8"/>
+      <c r="Q145" s="8"/>
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A146" s="13" t="s">
+      <c r="A146" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="B146" s="13" t="s">
+      <c r="B146" s="11" t="s">
         <v>298</v>
       </c>
-      <c r="C146" s="13"/>
-      <c r="D146" s="13"/>
-      <c r="E146" s="13"/>
-      <c r="F146" s="13"/>
-      <c r="G146" s="13"/>
-      <c r="H146" s="13"/>
-      <c r="I146" s="13"/>
-      <c r="J146" s="13"/>
-      <c r="K146" s="13"/>
-      <c r="L146" s="13"/>
-      <c r="M146" s="13"/>
-      <c r="N146" s="13"/>
-      <c r="O146" s="13"/>
-      <c r="P146" s="13"/>
-      <c r="Q146" s="13"/>
+      <c r="D146" s="8"/>
+      <c r="E146" s="8"/>
+      <c r="F146" s="8"/>
+      <c r="G146" s="8"/>
+      <c r="H146" s="8"/>
+      <c r="I146" s="8"/>
+      <c r="J146" s="8"/>
+      <c r="K146" s="8"/>
+      <c r="L146" s="8"/>
+      <c r="M146" s="8"/>
+      <c r="N146" s="8"/>
+      <c r="O146" s="8"/>
+      <c r="P146" s="8"/>
+      <c r="Q146" s="8"/>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A147" s="13" t="s">
+      <c r="A147" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="B147" s="13" t="s">
+      <c r="B147" s="11" t="s">
         <v>298</v>
       </c>
-      <c r="C147" s="13"/>
-      <c r="D147" s="13"/>
-      <c r="E147" s="13"/>
-      <c r="F147" s="13"/>
-      <c r="G147" s="13"/>
-      <c r="H147" s="13"/>
-      <c r="I147" s="13"/>
-      <c r="J147" s="13"/>
-      <c r="K147" s="13"/>
-      <c r="L147" s="13"/>
-      <c r="M147" s="13"/>
-      <c r="N147" s="13"/>
-      <c r="O147" s="13"/>
-      <c r="P147" s="13"/>
-      <c r="Q147" s="13"/>
+      <c r="D147" s="8"/>
+      <c r="E147" s="8"/>
+      <c r="F147" s="8"/>
+      <c r="G147" s="8"/>
+      <c r="H147" s="8"/>
+      <c r="I147" s="8"/>
+      <c r="J147" s="8"/>
+      <c r="K147" s="8"/>
+      <c r="L147" s="8"/>
+      <c r="M147" s="8"/>
+      <c r="N147" s="8"/>
+      <c r="O147" s="8"/>
+      <c r="P147" s="8"/>
+      <c r="Q147" s="8"/>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A148" s="14" t="s">
+      <c r="A148" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="B148" s="14" t="s">
+      <c r="B148" s="15" t="s">
         <v>291</v>
       </c>
-      <c r="C148" s="13"/>
-      <c r="D148" s="13"/>
-      <c r="E148" s="13"/>
-      <c r="F148" s="13"/>
-      <c r="G148" s="13"/>
-      <c r="H148" s="13"/>
-      <c r="I148" s="13"/>
-      <c r="J148" s="13"/>
-      <c r="K148" s="13"/>
-      <c r="L148" s="13"/>
-      <c r="M148" s="13"/>
-      <c r="N148" s="13"/>
-      <c r="O148" s="13"/>
-      <c r="P148" s="13"/>
-      <c r="Q148" s="13"/>
+      <c r="D148" s="8"/>
+      <c r="E148" s="8"/>
+      <c r="F148" s="8"/>
+      <c r="G148" s="8"/>
+      <c r="H148" s="8"/>
+      <c r="I148" s="8"/>
+      <c r="J148" s="8"/>
+      <c r="K148" s="8"/>
+      <c r="L148" s="8"/>
+      <c r="M148" s="8"/>
+      <c r="N148" s="8"/>
+      <c r="O148" s="8"/>
+      <c r="P148" s="8"/>
+      <c r="Q148" s="8"/>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A149" s="13" t="s">
+      <c r="A149" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="B149" s="13" t="s">
+      <c r="B149" s="11" t="s">
         <v>293</v>
       </c>
-      <c r="C149" s="13"/>
-      <c r="D149" s="13"/>
-      <c r="E149" s="13"/>
-      <c r="F149" s="13"/>
-      <c r="G149" s="13"/>
-      <c r="H149" s="13"/>
-      <c r="I149" s="13"/>
-      <c r="J149" s="13"/>
-      <c r="K149" s="13"/>
-      <c r="L149" s="13"/>
-      <c r="M149" s="13"/>
-      <c r="N149" s="13"/>
-      <c r="O149" s="13"/>
-      <c r="P149" s="13"/>
-      <c r="Q149" s="13"/>
+      <c r="D149" s="8"/>
+      <c r="E149" s="8"/>
+      <c r="F149" s="8"/>
+      <c r="G149" s="8"/>
+      <c r="H149" s="8"/>
+      <c r="I149" s="8"/>
+      <c r="J149" s="8"/>
+      <c r="K149" s="8"/>
+      <c r="L149" s="8"/>
+      <c r="M149" s="8"/>
+      <c r="N149" s="8"/>
+      <c r="O149" s="8"/>
+      <c r="P149" s="8"/>
+      <c r="Q149" s="8"/>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A150" s="13" t="s">
+      <c r="A150" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="B150" s="13" t="s">
+      <c r="B150" s="11" t="s">
         <v>295</v>
       </c>
-      <c r="C150" s="13"/>
-      <c r="D150" s="13"/>
-      <c r="E150" s="13"/>
-      <c r="F150" s="13"/>
-      <c r="G150" s="13"/>
-      <c r="H150" s="13"/>
-      <c r="I150" s="13"/>
-      <c r="J150" s="13"/>
-      <c r="K150" s="13"/>
-      <c r="L150" s="13"/>
-      <c r="M150" s="13"/>
-      <c r="N150" s="13"/>
-      <c r="O150" s="13"/>
-      <c r="P150" s="13"/>
-      <c r="Q150" s="13"/>
+      <c r="D150" s="8"/>
+      <c r="E150" s="8"/>
+      <c r="F150" s="8"/>
+      <c r="G150" s="8"/>
+      <c r="H150" s="8"/>
+      <c r="I150" s="8"/>
+      <c r="J150" s="8"/>
+      <c r="K150" s="8"/>
+      <c r="L150" s="8"/>
+      <c r="M150" s="8"/>
+      <c r="N150" s="8"/>
+      <c r="O150" s="8"/>
+      <c r="P150" s="8"/>
+      <c r="Q150" s="8"/>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A151" s="13" t="s">
+      <c r="A151" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="B151" s="13" t="s">
+      <c r="B151" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="C151" s="13"/>
-      <c r="D151" s="13"/>
-      <c r="E151" s="13"/>
-      <c r="F151" s="13"/>
-      <c r="G151" s="13"/>
-      <c r="H151" s="13"/>
-      <c r="I151" s="13"/>
-      <c r="J151" s="13"/>
-      <c r="K151" s="13"/>
-      <c r="L151" s="13"/>
-      <c r="M151" s="13"/>
-      <c r="N151" s="13"/>
-      <c r="O151" s="13"/>
-      <c r="P151" s="13"/>
-      <c r="Q151" s="13"/>
+      <c r="D151" s="8"/>
+      <c r="E151" s="8"/>
+      <c r="F151" s="8"/>
+      <c r="G151" s="8"/>
+      <c r="H151" s="8"/>
+      <c r="I151" s="8"/>
+      <c r="J151" s="8"/>
+      <c r="K151" s="8"/>
+      <c r="L151" s="8"/>
+      <c r="M151" s="8"/>
+      <c r="N151" s="8"/>
+      <c r="O151" s="8"/>
+      <c r="P151" s="8"/>
+      <c r="Q151" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>